<commit_message>
Results formatting + full data augmented.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\systemes\MusicMachineLearning\chord2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27110749-4782-470F-BD68-A9C0890C8F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1282180C-750A-4619-9357-79C2A2CCD87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>small</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Hidden Forest Embed</t>
   </si>
   <si>
-    <t>Pre-training</t>
-  </si>
-  <si>
     <t>model variant</t>
   </si>
   <si>
@@ -70,13 +67,22 @@
   </si>
   <si>
     <t>shuffle</t>
+  </si>
+  <si>
+    <t>lstm vanilla</t>
+  </si>
+  <si>
+    <t>Pretraining</t>
+  </si>
+  <si>
+    <t>Validation scores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,16 +90,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,17 +128,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60 % - Accent3" xfId="1" builtinId="40"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -122,6 +193,32 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1955AC10-F806-4383-AD69-1626383965D8}" name="Tableau3" displayName="Tableau3" ref="A2:E10" totalsRowShown="0">
+  <autoFilter ref="A2:E10" xr:uid="{1955AC10-F806-4383-AD69-1626383965D8}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A6CFC974-92EB-4BBC-A1AA-D979AED7056B}" name="model/dataset"/>
+    <tableColumn id="2" xr3:uid="{AB723984-481D-4D99-B294-441F890CA126}" name="model variant" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{8CF01639-3158-442A-8860-6B9EC1F298F9}" name="small"/>
+    <tableColumn id="4" xr3:uid="{4E31171F-9CC1-43CE-86CF-24E59C3EE41F}" name="medium"/>
+    <tableColumn id="5" xr3:uid="{5AA7B44E-3FA3-474B-AE64-0756EB99B561}" name="large"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}" name="Tableau6" displayName="Tableau6" ref="A14:C20" totalsRowShown="0">
+  <autoFilter ref="A14:C20" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8E56BF20-B978-4E6F-97A3-99DAB06302EA}" name="model/dataset"/>
+    <tableColumn id="2" xr3:uid="{34C0A48A-6CE4-4674-B031-729BCAB0C4F6}" name="model variant" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{5CE775DF-3749-4474-B13C-C304B9FC74EF}" name="small"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,121 +484,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>0</v>
-      </c>
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Set result pretraining phase 1
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,33 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\systemes\MusicMachineLearning\chord2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1282180C-750A-4619-9357-79C2A2CCD87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19A4C54-7F5C-48D5-B473-44352B2F2D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
-  <si>
-    <t>small</t>
-  </si>
-  <si>
-    <t>medium</t>
-  </si>
-  <si>
-    <t>large</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>model/dataset</t>
   </si>
@@ -51,9 +53,6 @@
     <t>model variant</t>
   </si>
   <si>
-    <t>lstm embed</t>
-  </si>
-  <si>
     <t>full window slide</t>
   </si>
   <si>
@@ -69,13 +68,31 @@
     <t>shuffle</t>
   </si>
   <si>
-    <t>lstm vanilla</t>
-  </si>
-  <si>
     <t>Pretraining</t>
   </si>
   <si>
-    <t>Validation scores</t>
+    <t>Embedding</t>
+  </si>
+  <si>
+    <t>Embedding augmented</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>small (%)</t>
+  </si>
+  <si>
+    <t>medium (%)</t>
+  </si>
+  <si>
+    <t>large (%)</t>
+  </si>
+  <si>
+    <t>Validation accuracy scores</t>
+  </si>
+  <si>
+    <t>LST Vanilla</t>
   </si>
 </sst>
 </file>
@@ -145,13 +162,13 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60 % - Accent3" xfId="1" builtinId="40"/>
@@ -201,21 +218,23 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A6CFC974-92EB-4BBC-A1AA-D979AED7056B}" name="model/dataset"/>
     <tableColumn id="2" xr3:uid="{AB723984-481D-4D99-B294-441F890CA126}" name="model variant" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{8CF01639-3158-442A-8860-6B9EC1F298F9}" name="small"/>
-    <tableColumn id="4" xr3:uid="{4E31171F-9CC1-43CE-86CF-24E59C3EE41F}" name="medium"/>
-    <tableColumn id="5" xr3:uid="{5AA7B44E-3FA3-474B-AE64-0756EB99B561}" name="large"/>
+    <tableColumn id="3" xr3:uid="{8CF01639-3158-442A-8860-6B9EC1F298F9}" name="small (%)"/>
+    <tableColumn id="4" xr3:uid="{4E31171F-9CC1-43CE-86CF-24E59C3EE41F}" name="medium (%)"/>
+    <tableColumn id="5" xr3:uid="{5AA7B44E-3FA3-474B-AE64-0756EB99B561}" name="large (%)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}" name="Tableau6" displayName="Tableau6" ref="A14:C20" totalsRowShown="0">
-  <autoFilter ref="A14:C20" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}" name="Tableau6" displayName="Tableau6" ref="A14:E22" totalsRowShown="0">
+  <autoFilter ref="A14:E22" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E56BF20-B978-4E6F-97A3-99DAB06302EA}" name="model/dataset"/>
     <tableColumn id="2" xr3:uid="{34C0A48A-6CE4-4674-B031-729BCAB0C4F6}" name="model variant" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{5CE775DF-3749-4474-B13C-C304B9FC74EF}" name="small"/>
+    <tableColumn id="3" xr3:uid="{5CE775DF-3749-4474-B13C-C304B9FC74EF}" name="small (%)"/>
+    <tableColumn id="4" xr3:uid="{16778C1F-672B-4334-9F5C-228C61DA2513}" name="medium (%)"/>
+    <tableColumn id="5" xr3:uid="{E0EF8084-0428-4CB6-934E-FDE157448131}" name="large (%)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -484,159 +503,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4"/>
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="s">
-        <v>12</v>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
-        <v>13</v>
+      <c r="B7" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4"/>
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
-        <v>12</v>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
-        <v>13</v>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="4"/>
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="B16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6">
+        <f>(0.0332 + 0.0421 + 0.0391) / 3 * 100</f>
+        <v>3.813333333333333</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="C17">
+        <f>(0.0307 + 0.019 + 0.0146) / 3 * 100</f>
+        <v>2.1433333333333331</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3"/>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Train for not augmented embeddings.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\systemes\MusicMachineLearning\chord2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19A4C54-7F5C-48D5-B473-44352B2F2D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F732DAF-EEA6-4869-A4D4-C418AB21224A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,7 +506,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,6 +676,10 @@
       <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C19">
+        <f>(0.0438 + 0.0412 + 0.0403) / 3 * 100</f>
+        <v>4.1766666666666667</v>
+      </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
@@ -687,6 +691,10 @@
       <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="C20">
+        <f>(0.0365 + 0.0322 + 0.0132) / 3 * 100</f>
+        <v>2.73</v>
+      </c>
       <c r="D20" t="s">
         <v>13</v>
       </c>
@@ -705,7 +713,10 @@
       <c r="D21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1">
+        <f>0.0998 * 100</f>
+        <v>9.98</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -718,7 +729,10 @@
       <c r="D22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1">
+        <f>0.1108*100</f>
+        <v>11.08</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Embed cbow path + results.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\systemes\MusicMachineLearning\chord2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455FFA71-E393-4B88-90FC-0A095D19BE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A48CE38-401F-4DE3-9174-7460ACC5B193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,7 +506,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,8 +730,8 @@
         <v>13</v>
       </c>
       <c r="E22" s="1">
-        <f>0.1108*100</f>
-        <v>11.08</v>
+        <f>(0.1108 + 0.1107)/2*100</f>
+        <v>11.074999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Results table for augmented and not augmented embeddings.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\systemes\MusicMachineLearning\chord2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A48CE38-401F-4DE3-9174-7460ACC5B193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBFC5AD-7B25-4046-A6C6-A5DDBE07E525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
   <si>
     <t>model/dataset</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>LST Vanilla</t>
+  </si>
+  <si>
+    <t>augmented data</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -123,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +142,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -155,11 +170,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
@@ -169,8 +185,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="20 % - Accent4" xfId="2" builtinId="42"/>
     <cellStyle name="60 % - Accent3" xfId="1" builtinId="40"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -213,11 +234,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1955AC10-F806-4383-AD69-1626383965D8}" name="Tableau3" displayName="Tableau3" ref="A2:E10" totalsRowShown="0">
-  <autoFilter ref="A2:E10" xr:uid="{1955AC10-F806-4383-AD69-1626383965D8}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1955AC10-F806-4383-AD69-1626383965D8}" name="Tableau3" displayName="Tableau3" ref="A2:F22" totalsRowShown="0">
+  <autoFilter ref="A2:F22" xr:uid="{1955AC10-F806-4383-AD69-1626383965D8}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A6CFC974-92EB-4BBC-A1AA-D979AED7056B}" name="model/dataset"/>
-    <tableColumn id="2" xr3:uid="{AB723984-481D-4D99-B294-441F890CA126}" name="model variant" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{AB723984-481D-4D99-B294-441F890CA126}" name="model variant"/>
+    <tableColumn id="6" xr3:uid="{280E5A6E-0C74-48D7-AD87-B6FCC8BC4DDB}" name="augmented data" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{8CF01639-3158-442A-8860-6B9EC1F298F9}" name="small (%)"/>
     <tableColumn id="4" xr3:uid="{4E31171F-9CC1-43CE-86CF-24E59C3EE41F}" name="medium (%)"/>
     <tableColumn id="5" xr3:uid="{5AA7B44E-3FA3-474B-AE64-0756EB99B561}" name="large (%)"/>
@@ -227,11 +249,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}" name="Tableau6" displayName="Tableau6" ref="A14:E22" totalsRowShown="0">
-  <autoFilter ref="A14:E22" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}" name="Tableau6" displayName="Tableau6" ref="A26:E34" totalsRowShown="0">
+  <autoFilter ref="A26:E34" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E56BF20-B978-4E6F-97A3-99DAB06302EA}" name="model/dataset"/>
-    <tableColumn id="2" xr3:uid="{34C0A48A-6CE4-4674-B031-729BCAB0C4F6}" name="model variant" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{34C0A48A-6CE4-4674-B031-729BCAB0C4F6}" name="model variant" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{5CE775DF-3749-4474-B13C-C304B9FC74EF}" name="small (%)"/>
     <tableColumn id="4" xr3:uid="{16778C1F-672B-4334-9F5C-228C61DA2513}" name="medium (%)"/>
     <tableColumn id="5" xr3:uid="{E0EF8084-0428-4CB6-934E-FDE157448131}" name="large (%)"/>
@@ -503,22 +525,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -527,7 +549,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -535,208 +557,319 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>0</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C26" t="s">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D26" t="s">
         <v>15</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C28" s="6">
         <f>(0.0332 + 0.0421 + 0.0391) / 3 * 100</f>
         <v>3.813333333333333</v>
       </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C17">
+      <c r="C29">
         <f>(0.0307 + 0.019 + 0.0146) / 3 * 100</f>
         <v>2.1433333333333331</v>
       </c>
-      <c r="D17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C19">
+      <c r="C31">
         <f>(0.0438 + 0.0412 + 0.0403) / 3 * 100</f>
         <v>4.1766666666666667</v>
       </c>
-      <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C20">
+      <c r="C32">
         <f>(0.0365 + 0.0322 + 0.0132) / 3 * 100</f>
         <v>2.73</v>
       </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="B33" s="3"/>
+      <c r="C33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="1">
         <f>(0.0998 + 0.0995 )/2 * 100</f>
         <v>9.9649999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="B34" s="3"/>
+      <c r="C34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="1">
         <f>(0.1108 + 0.1107)/2*100</f>
         <v>11.074999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A25:C25"/>
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update results pre training.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\systemes\MusicMachineLearning\chord2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C086CB9-A769-41FE-9BF3-D6CC041802C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D924A7-F9EA-4F34-9846-5267FDC01727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
   <si>
     <t>model/dataset</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>embedding augmented</t>
+  </si>
+  <si>
+    <t>data augmented</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
@@ -184,7 +187,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
@@ -239,7 +241,7 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A6CFC974-92EB-4BBC-A1AA-D979AED7056B}" name="model/dataset"/>
     <tableColumn id="2" xr3:uid="{AB723984-481D-4D99-B294-441F890CA126}" name="model variant"/>
-    <tableColumn id="6" xr3:uid="{280E5A6E-0C74-48D7-AD87-B6FCC8BC4DDB}" name="embedding augmented" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{280E5A6E-0C74-48D7-AD87-B6FCC8BC4DDB}" name="embedding augmented" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{8CF01639-3158-442A-8860-6B9EC1F298F9}" name="small (%)"/>
     <tableColumn id="4" xr3:uid="{4E31171F-9CC1-43CE-86CF-24E59C3EE41F}" name="medium (%)"/>
     <tableColumn id="5" xr3:uid="{5AA7B44E-3FA3-474B-AE64-0756EB99B561}" name="large (%)"/>
@@ -249,11 +251,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}" name="Tableau6" displayName="Tableau6" ref="A26:E34" totalsRowShown="0">
-  <autoFilter ref="A26:E34" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}" name="Tableau6" displayName="Tableau6" ref="A26:F42" totalsRowShown="0">
+  <autoFilter ref="A26:F42" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{8E56BF20-B978-4E6F-97A3-99DAB06302EA}" name="model/dataset"/>
-    <tableColumn id="2" xr3:uid="{34C0A48A-6CE4-4674-B031-729BCAB0C4F6}" name="model variant" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{34C0A48A-6CE4-4674-B031-729BCAB0C4F6}" name="model variant"/>
+    <tableColumn id="6" xr3:uid="{7AF8BE0F-F291-4E82-BE2D-9C4362DE337B}" name="data augmented" dataDxfId="0" dataCellStyle="60 % - Accent3"/>
     <tableColumn id="3" xr3:uid="{5CE775DF-3749-4474-B13C-C304B9FC74EF}" name="small (%)"/>
     <tableColumn id="4" xr3:uid="{16778C1F-672B-4334-9F5C-228C61DA2513}" name="medium (%)"/>
     <tableColumn id="5" xr3:uid="{E0EF8084-0428-4CB6-934E-FDE157448131}" name="large (%)"/>
@@ -525,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,15 +583,15 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
@@ -604,15 +607,15 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
@@ -628,49 +631,49 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
@@ -686,49 +689,49 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="4" t="s">
         <v>20</v>
       </c>
@@ -748,12 +751,15 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
         <v>14</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>15</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>16</v>
       </c>
     </row>
@@ -761,108 +767,192 @@
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29">
         <f>(0.0332 + 0.0421 + 0.0391) / 3 * 100</f>
         <v>3.813333333333333</v>
       </c>
-      <c r="D28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C29">
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32">
         <f>(0.0307 + 0.019 + 0.0146) / 3 * 100</f>
         <v>2.1433333333333331</v>
       </c>
-      <c r="D29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C31">
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36">
         <f>(0.0438 + 0.0412 + 0.0403) / 3 * 100</f>
         <v>4.1766666666666667</v>
       </c>
-      <c r="D31" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C32">
+      <c r="C38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39">
         <f>(0.0365 + 0.0322 + 0.0132) / 3 * 100</f>
         <v>2.73</v>
       </c>
-      <c r="D32" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="1">
+      <c r="B41" s="2"/>
+      <c r="C41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="1">
         <f>(0.0998 + 0.0995 )/2 * 100</f>
         <v>9.9649999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="B42" s="2"/>
+      <c r="C42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="1">
         <f>(0.1108 + 0.1107)/2*100</f>
         <v>11.074999999999999</v>
       </c>

</xml_diff>

<commit_message>
Added pre training results.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\systemes\MusicMachineLearning\chord2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D924A7-F9EA-4F34-9846-5267FDC01727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E1CE7E-14F6-42B7-8BA6-A009725E2001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="23">
   <si>
     <t>model/dataset</t>
   </si>
@@ -251,8 +251,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}" name="Tableau6" displayName="Tableau6" ref="A26:F42" totalsRowShown="0">
-  <autoFilter ref="A26:F42" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}" name="Tableau6" displayName="Tableau6" ref="A26:F47" totalsRowShown="0">
+  <autoFilter ref="A26:F47" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{8E56BF20-B978-4E6F-97A3-99DAB06302EA}" name="model/dataset"/>
     <tableColumn id="2" xr3:uid="{34C0A48A-6CE4-4674-B031-729BCAB0C4F6}" name="model variant"/>
@@ -528,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,6 +806,16 @@
       <c r="C30" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="D30">
+        <f>(0.0911 + 0.0813 + 0.0878)/3 * 100</f>
+        <v>8.673333333333332</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
@@ -839,6 +849,16 @@
       <c r="B33" s="6"/>
       <c r="C33" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="D33">
+        <f>(0.0602 + 0.0451 + 0.0647) / 3 * 100</f>
+        <v>5.6666666666666661</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -884,6 +904,16 @@
       <c r="C37" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="D37">
+        <f>(0.0954 + 0.0817 + 0.0914)/3 * 100</f>
+        <v>8.9499999999999975</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
@@ -895,7 +925,7 @@
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="4" t="s">
@@ -918,41 +948,133 @@
       <c r="C40" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="D40">
+        <f>(0.0992 + 0.0887 + 0.0977) / 3 * 100</f>
+        <v>9.5200000000000014</v>
+      </c>
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="1">
+      <c r="B48" s="2"/>
+      <c r="C48" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="1">
         <f>(0.0998 + 0.0995 )/2 * 100</f>
         <v>9.9649999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="1">
+      <c r="B49" s="2"/>
+      <c r="C49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="1">
         <f>(0.1108 + 0.1107)/2*100</f>
         <v>11.074999999999999</v>
       </c>

</xml_diff>

<commit_message>
Pre training results finish.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\systemes\MusicMachineLearning\chord2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E1CE7E-14F6-42B7-8BA6-A009725E2001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16948459-B78B-4056-B06D-96371173AC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,6 +985,10 @@
       <c r="C43" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="D43">
+        <f>(0.496904024767801 + 0.496904024767801 + 0.461300309597523) / 3 * 100</f>
+        <v>48.503611971104171</v>
+      </c>
       <c r="E43" t="s">
         <v>13</v>
       </c>
@@ -998,6 +1002,10 @@
       <c r="C44" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="D44">
+        <f>(0.434715346534653 + 0.435334158415841 + 0.426980198019801) / 3 * 100</f>
+        <v>43.234323432343167</v>
+      </c>
       <c r="E44" t="s">
         <v>13</v>
       </c>
@@ -1021,6 +1029,10 @@
       <c r="C46" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="D46">
+        <f>(0.32824427480916 + 0.3206106870229 + 0.396946564885496) / 3 * 100</f>
+        <v>34.8600508905852</v>
+      </c>
       <c r="E46" t="s">
         <v>13</v>
       </c>
@@ -1033,6 +1045,10 @@
       <c r="B47" s="6"/>
       <c r="C47" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="D47">
+        <f>(0.266768292682926 + 0.265243902439024 +  0.271341463414634) / 3 * 100</f>
+        <v>26.778455284552805</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Start of training loop to iterate results + better results.xlsx
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\systemes\MusicMachineLearning\chord2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16948459-B78B-4056-B06D-96371173AC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9FA6D6-0D2E-421F-B4D3-10D879252899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,6 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,75 +33,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="23">
+  <si>
+    <t>Validation accuracy scores</t>
+  </si>
   <si>
     <t>model/dataset</t>
   </si>
   <si>
+    <t>model variant</t>
+  </si>
+  <si>
+    <t>embedding augmented</t>
+  </si>
+  <si>
+    <t>small (%)</t>
+  </si>
+  <si>
+    <t>medium (%)</t>
+  </si>
+  <si>
+    <t>large (%)</t>
+  </si>
+  <si>
     <t>LSTM Embed</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>LST Vanilla</t>
+  </si>
+  <si>
+    <t>Hidden Forest Embed</t>
+  </si>
+  <si>
+    <t>no shuffle</t>
+  </si>
+  <si>
+    <t>shuffle</t>
+  </si>
+  <si>
+    <t>Hidden Forest Vanilla</t>
+  </si>
+  <si>
+    <t>Pretraining</t>
+  </si>
+  <si>
+    <t>data augmented</t>
+  </si>
+  <si>
+    <t>overlap window slide</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>full window slide</t>
+  </si>
+  <si>
     <t>LSTM Vanilla</t>
   </si>
   <si>
-    <t>Hidden Forest Embed</t>
-  </si>
-  <si>
-    <t>model variant</t>
-  </si>
-  <si>
-    <t>full window slide</t>
-  </si>
-  <si>
-    <t>overlap window slide</t>
-  </si>
-  <si>
-    <t>Hidden Forest Vanilla</t>
-  </si>
-  <si>
-    <t>no shuffle</t>
-  </si>
-  <si>
-    <t>shuffle</t>
-  </si>
-  <si>
-    <t>Pretraining</t>
-  </si>
-  <si>
     <t>Embedding</t>
   </si>
   <si>
     <t>Embedding augmented</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>small (%)</t>
-  </si>
-  <si>
-    <t>medium (%)</t>
-  </si>
-  <si>
-    <t>large (%)</t>
-  </si>
-  <si>
-    <t>Validation accuracy scores</t>
-  </si>
-  <si>
-    <t>LST Vanilla</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>embedding augmented</t>
-  </si>
-  <si>
-    <t>data augmented</t>
   </si>
 </sst>
 </file>
@@ -175,22 +172,20 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20 % - Accent4" xfId="2" builtinId="42"/>
@@ -199,7 +194,7 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -211,7 +206,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -236,30 +231,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1955AC10-F806-4383-AD69-1626383965D8}" name="Tableau3" displayName="Tableau3" ref="A2:F22" totalsRowShown="0">
-  <autoFilter ref="A2:F22" xr:uid="{1955AC10-F806-4383-AD69-1626383965D8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau3" displayName="Tableau3" ref="A2:F22" totalsRowShown="0">
+  <autoFilter ref="A2:F22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A6CFC974-92EB-4BBC-A1AA-D979AED7056B}" name="model/dataset"/>
-    <tableColumn id="2" xr3:uid="{AB723984-481D-4D99-B294-441F890CA126}" name="model variant"/>
-    <tableColumn id="6" xr3:uid="{280E5A6E-0C74-48D7-AD87-B6FCC8BC4DDB}" name="embedding augmented" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{8CF01639-3158-442A-8860-6B9EC1F298F9}" name="small (%)"/>
-    <tableColumn id="4" xr3:uid="{4E31171F-9CC1-43CE-86CF-24E59C3EE41F}" name="medium (%)"/>
-    <tableColumn id="5" xr3:uid="{5AA7B44E-3FA3-474B-AE64-0756EB99B561}" name="large (%)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="model/dataset"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="model variant"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="embedding augmented" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="small (%)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="medium (%)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="large (%)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}" name="Tableau6" displayName="Tableau6" ref="A26:F47" totalsRowShown="0">
-  <autoFilter ref="A26:F47" xr:uid="{E4692D24-B73C-4339-AAB8-0E66DC10BA2B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau6" displayName="Tableau6" ref="A26:F54" totalsRowShown="0">
+  <autoFilter ref="A26:F54" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8E56BF20-B978-4E6F-97A3-99DAB06302EA}" name="model/dataset"/>
-    <tableColumn id="2" xr3:uid="{34C0A48A-6CE4-4674-B031-729BCAB0C4F6}" name="model variant"/>
-    <tableColumn id="6" xr3:uid="{7AF8BE0F-F291-4E82-BE2D-9C4362DE337B}" name="data augmented" dataDxfId="0" dataCellStyle="60 % - Accent3"/>
-    <tableColumn id="3" xr3:uid="{5CE775DF-3749-4474-B13C-C304B9FC74EF}" name="small (%)"/>
-    <tableColumn id="4" xr3:uid="{16778C1F-672B-4334-9F5C-228C61DA2513}" name="medium (%)"/>
-    <tableColumn id="5" xr3:uid="{E0EF8084-0428-4CB6-934E-FDE157448131}" name="large (%)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="model/dataset"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="model variant"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="data augmented" dataDxfId="0" dataCellStyle="60 % - Accent3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="small (%)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="medium (%)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="large (%)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -528,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,554 +538,596 @@
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+    <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="4" t="s">
-        <v>19</v>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="4" t="s">
-        <v>19</v>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="4" t="s">
-        <v>20</v>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="4" t="s">
-        <v>19</v>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="4" t="s">
-        <v>20</v>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="4" t="s">
-        <v>19</v>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="4" t="s">
-        <v>20</v>
+      <c r="C15" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="4" t="s">
-        <v>19</v>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="4" t="s">
-        <v>20</v>
+      <c r="C19" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="4" t="s">
-        <v>19</v>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
         <v>4</v>
       </c>
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" t="s">
-        <v>14</v>
-      </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
+      <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="2"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="4" t="s">
-        <v>19</v>
+      <c r="C29" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D29">
         <f>(0.0332 + 0.0421 + 0.0391) / 3 * 100</f>
         <v>3.813333333333333</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F29" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="4" t="s">
-        <v>20</v>
+      <c r="C30" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D30">
         <f>(0.0911 + 0.0813 + 0.0878)/3 * 100</f>
         <v>8.673333333333332</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="4" t="s">
-        <v>19</v>
+      <c r="C32" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D32">
         <f>(0.0307 + 0.019 + 0.0146) / 3 * 100</f>
         <v>2.1433333333333331</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F32" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="4" t="s">
-        <v>20</v>
+      <c r="C33" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D33">
         <f>(0.0602 + 0.0451 + 0.0647) / 3 * 100</f>
         <v>5.6666666666666661</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F33" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
+      <c r="A34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="2"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="4" t="s">
-        <v>19</v>
+      <c r="C36" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D36">
         <f>(0.0438 + 0.0412 + 0.0403) / 3 * 100</f>
         <v>4.1766666666666667</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F36" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="4" t="s">
-        <v>20</v>
+      <c r="C37" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D37">
         <f>(0.0954 + 0.0817 + 0.0914)/3 * 100</f>
         <v>8.9499999999999975</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F37" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="4" t="s">
-        <v>19</v>
+      <c r="C39" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D39">
         <f>(0.0365 + 0.0322 + 0.0132) / 3 * 100</f>
         <v>2.73</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F39" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="4" t="s">
-        <v>20</v>
+      <c r="C40" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D40">
         <f>(0.0992 + 0.0887 + 0.0977) / 3 * 100</f>
         <v>9.5200000000000014</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F40" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="3"/>
+      <c r="A41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="2"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="4" t="s">
-        <v>19</v>
+      <c r="C43" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D43">
         <f>(0.496904024767801 + 0.496904024767801 + 0.461300309597523) / 3 * 100</f>
         <v>48.503611971104171</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F43" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="4" t="s">
-        <v>20</v>
+      <c r="C44" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D44">
         <f>(0.434715346534653 + 0.435334158415841 + 0.426980198019801) / 3 * 100</f>
         <v>43.234323432343167</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F44" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="4" t="s">
-        <v>19</v>
+      <c r="C46" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D46">
-        <f>(0.32824427480916 + 0.3206106870229 + 0.396946564885496) / 3 * 100</f>
-        <v>34.8600508905852</v>
+        <f>(0.351145038167938 + 0.297709923664122 + 0.282442748091603 + 0.290076335877862 + 0.374045801526717) / 5 * 100</f>
+        <v>31.908396946564839</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F46" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="4" t="s">
-        <v>20</v>
+      <c r="C47" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D47">
         <f>(0.266768292682926 + 0.265243902439024 +  0.271341463414634) / 3 * 100</f>
         <v>26.778455284552805</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F47" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="3" t="s">
+      <c r="A48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <f>(0.496904024767801 + 0.496904024767801 + 0.461300309597523) / 3 * 100</f>
+        <v>48.503611971104171</v>
+      </c>
+      <c r="E50" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51">
+        <f>(0.434715346534653 + 0.435334158415841 + 0.426980198019801) / 3 * 100</f>
+        <v>43.234323432343167</v>
+      </c>
+      <c r="E51" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F48" s="1">
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53">
+        <f>(0.351145038167938 + 0.297709923664122 + 0.282442748091603 + 0.290076335877862 + 0.374045801526717) / 5 * 100</f>
+        <v>31.908396946564839</v>
+      </c>
+      <c r="E53" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54">
+        <f>(0.266768292682926 + 0.265243902439024 +  0.271341463414634) / 3 * 100</f>
+        <v>26.778455284552805</v>
+      </c>
+      <c r="E54" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" s="1">
         <f>(0.0998 + 0.0995 )/2 * 100</f>
         <v>9.9649999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="1">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" s="1">
         <f>(0.1108 + 0.1107)/2*100</f>
         <v>11.074999999999999</v>
       </c>
@@ -1101,10 +1138,10 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First pre train run.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\systemes\MusicMachineLearning\chord2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9FA6D6-0D2E-421F-B4D3-10D879252899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6DE9BE-59F0-42E3-84E8-9EFBE151766B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,8 +759,8 @@
         <v>8</v>
       </c>
       <c r="D29">
-        <f>(0.0332 + 0.0421 + 0.0391) / 3 * 100</f>
-        <v>3.813333333333333</v>
+        <f>(0.0409356725146198 + 0.0487329434697855 + 0.0487329434697855 + 0.0526315789473684 + 0.0448343079922027) / 5 * 100</f>
+        <v>4.7173489278752383</v>
       </c>
       <c r="E29" t="s">
         <v>18</v>
@@ -774,8 +774,8 @@
         <v>9</v>
       </c>
       <c r="D30">
-        <f>(0.0911 + 0.0813 + 0.0878)/3 * 100</f>
-        <v>8.673333333333332</v>
+        <f>(0.0892966360856269 + 0.0951070336391437 + 0.0938837920489296 + 0.0889908256880734 + 0.0954128440366972) / 5 * 100</f>
+        <v>9.2538226299694166</v>
       </c>
       <c r="E30" t="s">
         <v>18</v>
@@ -799,8 +799,8 @@
         <v>8</v>
       </c>
       <c r="D32">
-        <f>(0.0307 + 0.019 + 0.0146) / 3 * 100</f>
-        <v>2.1433333333333331</v>
+        <f>(0.019047619047619 + 0.0380952380952381 + 0.0285714285714285 + 0.0285714285714285 + 0.019047619047619) / 5 * 100</f>
+        <v>2.6666666666666625</v>
       </c>
       <c r="E32" t="s">
         <v>18</v>
@@ -814,8 +814,8 @@
         <v>9</v>
       </c>
       <c r="D33">
-        <f>(0.0602 + 0.0451 + 0.0647) / 3 * 100</f>
-        <v>5.6666666666666661</v>
+        <f>(0.0902255639097744 + 0.0796992481203007 + 0.0736842105263157 + 0.0721804511278195 + 0.069172932330827) / 5 * 100</f>
+        <v>7.6992481203007461</v>
       </c>
       <c r="E33" t="s">
         <v>18</v>
@@ -849,8 +849,8 @@
         <v>8</v>
       </c>
       <c r="D36">
-        <f>(0.0438 + 0.0412 + 0.0403) / 3 * 100</f>
-        <v>4.1766666666666667</v>
+        <f>(0.0175438596491228 + 0.0584795321637426 + 0.0487329434697855 + 0.0253411306042884 + 0.0389863547758284) / 5 * 100</f>
+        <v>3.781676413255354</v>
       </c>
       <c r="E36" t="s">
         <v>18</v>
@@ -864,8 +864,8 @@
         <v>9</v>
       </c>
       <c r="D37">
-        <f>(0.0954 + 0.0817 + 0.0914)/3 * 100</f>
-        <v>8.9499999999999975</v>
+        <f>(0.091131498470948 + 0.0877675840978593 + 0.0856269113149847 + 0.0877675840978593 + 0.0963302752293578) / 5 * 100</f>
+        <v>8.9724770642201808</v>
       </c>
       <c r="E37" t="s">
         <v>18</v>
@@ -889,8 +889,8 @@
         <v>8</v>
       </c>
       <c r="D39">
-        <f>(0.0365 + 0.0322 + 0.0132) / 3 * 100</f>
-        <v>2.73</v>
+        <f>(0.00952380952380952 + 0.0285714285714285 + 0.0380952380952381 + 0.0476190476190476 + 0.0571428571428571) / 5 * 100</f>
+        <v>3.619047619047616</v>
       </c>
       <c r="E39" t="s">
         <v>18</v>
@@ -904,8 +904,8 @@
         <v>9</v>
       </c>
       <c r="D40">
-        <f>(0.0992 + 0.0887 + 0.0977) / 3 * 100</f>
-        <v>9.5200000000000014</v>
+        <f>(0.0796992481203007 + 0.0857142857142857 + 0.0827067669172932 + 0.0947368421052631 + 0.0887218045112782) / 5 * 100</f>
+        <v>8.6315789473684177</v>
       </c>
       <c r="E40" t="s">
         <v>18</v>
@@ -939,8 +939,8 @@
         <v>8</v>
       </c>
       <c r="D43">
-        <f>(0.496904024767801 + 0.496904024767801 + 0.461300309597523) / 3 * 100</f>
-        <v>48.503611971104171</v>
+        <f>(0.490712074303405 + 0.467492260061919 + 0.530959752321981 + 0.507739938080495 + 0.5) / 5 * 100</f>
+        <v>49.938080495356004</v>
       </c>
       <c r="E43" t="s">
         <v>18</v>
@@ -954,8 +954,8 @@
         <v>9</v>
       </c>
       <c r="D44">
-        <f>(0.434715346534653 + 0.435334158415841 + 0.426980198019801) / 3 * 100</f>
-        <v>43.234323432343167</v>
+        <f>(0.446163366336633 + 0.441212871287128 + 0.435024752475247 + 0.430074257425742 + 0.440903465346534) / 5 * 100</f>
+        <v>43.86757425742568</v>
       </c>
       <c r="E44" t="s">
         <v>18</v>
@@ -979,8 +979,8 @@
         <v>8</v>
       </c>
       <c r="D46">
-        <f>(0.351145038167938 + 0.297709923664122 + 0.282442748091603 + 0.290076335877862 + 0.374045801526717) / 5 * 100</f>
-        <v>31.908396946564839</v>
+        <f>(0.305343511450381 + 0.358778625954198 + 0.32824427480916 + 0.312977099236641 + 0.343511450381679) / 5 * 100</f>
+        <v>32.97709923664118</v>
       </c>
       <c r="E46" t="s">
         <v>18</v>
@@ -994,8 +994,8 @@
         <v>9</v>
       </c>
       <c r="D47">
-        <f>(0.266768292682926 + 0.265243902439024 +  0.271341463414634) / 3 * 100</f>
-        <v>26.778455284552805</v>
+        <f>(0.278963414634146 + 0.234756097560975 + 0.28810975609756 + 0.268292682926829 + 0.283536585365853) / 5 * 100</f>
+        <v>27.073170731707265</v>
       </c>
       <c r="E47" t="s">
         <v>18</v>
@@ -1029,8 +1029,8 @@
         <v>8</v>
       </c>
       <c r="D50">
-        <f>(0.496904024767801 + 0.496904024767801 + 0.461300309597523) / 3 * 100</f>
-        <v>48.503611971104171</v>
+        <f>(0.41640866873065 + 0.455108359133126 + 0.439628482972136 + 0.411764705882352 + 0.452012383900928) / 5 * 100</f>
+        <v>43.498452012383844</v>
       </c>
       <c r="E50" t="s">
         <v>18</v>
@@ -1044,8 +1044,8 @@
         <v>9</v>
       </c>
       <c r="D51">
-        <f>(0.434715346534653 + 0.435334158415841 + 0.426980198019801) / 3 * 100</f>
-        <v>43.234323432343167</v>
+        <f>(0.398205445544554 + 0.394183168316831 + 0.392017326732673 + 0.395111386138613 + 0.39789603960396) / 5 * 100</f>
+        <v>39.548267326732613</v>
       </c>
       <c r="E51" t="s">
         <v>18</v>
@@ -1069,8 +1069,8 @@
         <v>8</v>
       </c>
       <c r="D53">
-        <f>(0.351145038167938 + 0.297709923664122 + 0.282442748091603 + 0.290076335877862 + 0.374045801526717) / 5 * 100</f>
-        <v>31.908396946564839</v>
+        <f>(0.229007633587786 + 0.206106870229007 + 0.221374045801526 + 0.305343511450381 + 0.297709923664122) / 5 * 100</f>
+        <v>25.190839694656443</v>
       </c>
       <c r="E53" t="s">
         <v>18</v>
@@ -1084,8 +1084,8 @@
         <v>9</v>
       </c>
       <c r="D54">
-        <f>(0.266768292682926 + 0.265243902439024 +  0.271341463414634) / 3 * 100</f>
-        <v>26.778455284552805</v>
+        <f>(0.216463414634146 + 0.204268292682926 + 0.213414634146341 + 0.236280487804878 + 0.198170731707317) / 5 * 100</f>
+        <v>21.371951219512159</v>
       </c>
       <c r="E54" t="s">
         <v>18</v>
@@ -1109,8 +1109,8 @@
         <v>18</v>
       </c>
       <c r="F55" s="1">
-        <f>(0.0998 + 0.0995 )/2 * 100</f>
-        <v>9.9649999999999999</v>
+        <f>(0.0993930197268588) / 1 * 100</f>
+        <v>9.9393019726858789</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1128,8 +1128,8 @@
         <v>18</v>
       </c>
       <c r="F56" s="1">
-        <f>(0.1108 + 0.1107)/2*100</f>
-        <v>11.074999999999999</v>
+        <f>(0.11067476294194) / 1 * 100</f>
+        <v>11.067476294194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added color highlights to data.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\systemes\MusicMachineLearning\chord2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A5DF53-F0AF-4E55-800C-02E5B195C403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526A422C-0A5B-4747-8493-820042815B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,8 +131,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +171,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -182,14 +202,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
@@ -202,12 +224,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="20 % - Accent1" xfId="3" builtinId="30"/>
     <cellStyle name="20 % - Accent2" xfId="4" builtinId="34"/>
     <cellStyle name="20 % - Accent4" xfId="2" builtinId="42"/>
+    <cellStyle name="40 % - Accent5" xfId="5" builtinId="47"/>
     <cellStyle name="60 % - Accent3" xfId="1" builtinId="40"/>
+    <cellStyle name="60 % - Accent6" xfId="6" builtinId="52"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -557,7 +585,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,9 +687,9 @@
       <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6">
-        <f>(0.082874617737003 + 0.0807339449541284 + 0.091131498470948 + 0.0837920489296636 + 0.0862385321100917) / 5 * 100</f>
-        <v>8.4954128440366947</v>
+      <c r="E6" s="11">
+        <f>(0.0526315789473684 + 0.0389863547758284 + 0.0487329434697855 + 0.0721247563352826 + 0.0487329434697855) / 5 * 100</f>
+        <v>5.2241715399610076</v>
       </c>
       <c r="F6">
         <f>(0.117907980722958 + 0.119958433008097 + 0.119170334000544) / 3 * 100</f>
@@ -679,15 +707,15 @@
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="10">
         <f>(0.0862385321100917 + 0.0868501529051987 + 0.0743119266055045 + 0.0938837920489296 + 0.0819571865443425) / 5 * 100</f>
         <v>8.4648318042813404</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="12">
         <f>(0.122622626113277 + 0.122992265470801 + 0.123013188453303) / 3 * 100</f>
         <v>12.287602667912701</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="12">
         <f>(0.207610489229808) / 1 * 100</f>
         <v>20.761048922980798</v>
       </c>
@@ -738,15 +766,15 @@
       <c r="D11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="12">
         <f>(0.0892966360856269 + 0.0993883792048929 + 0.0892966360856269 + 0.0954128440366972 + 0.0972477064220183) / 5 * 100</f>
         <v>9.4128440366972441</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="10">
         <f>(0.0908615386761331 + 0.0919913797312094 + 0.118549618853002) / 3 * 100</f>
         <v>10.046751242011483</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="10">
         <f>(0.168997234981938) / 1 * 100</f>
         <v>16.899723498193801</v>
       </c>
@@ -816,7 +844,7 @@
         <f>(0.125072236440188 + 0.128126805911004 + 0.123751341533889) / 3 * 100</f>
         <v>12.565012796169366</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="10">
         <f>(0.154936395361927) / 1 * 100</f>
         <v>15.493639536192699</v>
       </c>
@@ -844,11 +872,11 @@
       <c r="D18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="10">
         <f>(0.230412071967498 + 0.233894370284387 + 0.233313987231572 + 0.230992455020313 + 0.233313987231572) / 5 * 100</f>
         <v>23.238537434706839</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="10">
         <f>(0.15608495495241 + 0.155647188409071 + 0.159121077752986) / 3 * 100</f>
         <v>15.695107370482233</v>
       </c>
@@ -871,15 +899,15 @@
       <c r="D20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="13">
         <f>(0.490712074303405 + 0.5 + 0.5 + 0.484520123839009 + 0.517027863777089) / 5 * 100</f>
         <v>49.845201238390061</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="13">
         <f>(0.593144401379653 + 0.590619777406393 + 0.591153148668349) / 3 * 100</f>
         <v>59.163910915146502</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="13">
         <f>(0.512935858087819) / 1 * 100</f>
         <v>51.293585808781906</v>
       </c>
@@ -993,7 +1021,7 @@
         <f>(0.0984066705192768 + 0.102534467101461 + 0.103690250144472) / 3 * 100</f>
         <v>10.154379592173662</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="10">
         <f>(0.131419565462118) / 1 * 100</f>
         <v>13.1419565462118</v>
       </c>
@@ -1009,7 +1037,7 @@
         <f>(0.195008705745792 + 0.191526407428903 + 0.194428322692977 + 0.188044109112013 + 0.196749854904236) / 5 * 100</f>
         <v>19.315147997678423</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="10">
         <f>(0.128548027226254 + 0.12957889682831 + 0.128152625187109) / 3 * 100</f>
         <v>12.875984974722432</v>
       </c>
@@ -1021,7 +1049,7 @@
       <c r="D29" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="10">
         <f>(0.190946024376088 + 0.20081253627394 + 0.196749854904236 + 0.190365641323273 + 0.194428322692977) / 5 * 100</f>
         <v>19.46604759141028</v>
       </c>
@@ -1048,15 +1076,15 @@
       <c r="D31" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="10">
         <f>(0.391640866873065 + 0.430340557275541 + 0.44891640866873 + 0.455108359133126 + 0.442724458204334) / 5 * 100</f>
         <v>43.374613003095916</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="10">
         <f>(0.54795007644988 + 0.553497137574227 + 0.550830281264445) / 3 * 100</f>
         <v>55.075916509618409</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="10">
         <f>(0.483374513866575) / 1 * 100</f>
         <v>48.337451386657499</v>
       </c>
@@ -1545,10 +1573,10 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>